<commit_message>
score_matchup seems to work now? lots more testing required
</commit_message>
<xml_diff>
--- a/data/stats.xlsx
+++ b/data/stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544" uniqueCount="711">
   <si>
     <t>Index</t>
   </si>
@@ -2132,6 +2132,9 @@
   </si>
   <si>
     <t>S Florida</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
   <si>
     <t>DIVISION 1  FBS</t>
@@ -2562,7 +2565,7 @@
         <v>82.2</v>
       </c>
       <c r="G2" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H2">
         <v>0.336</v>
@@ -2597,7 +2600,7 @@
         <v>84.2</v>
       </c>
       <c r="G3" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H3">
         <v>0.302</v>
@@ -2632,7 +2635,7 @@
         <v>83.90000000000001</v>
       </c>
       <c r="G4" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H4">
         <v>0.325</v>
@@ -2667,7 +2670,7 @@
         <v>86.59999999999999</v>
       </c>
       <c r="G5" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H5">
         <v>0.197</v>
@@ -2702,7 +2705,7 @@
         <v>109.5</v>
       </c>
       <c r="G6" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H6">
         <v>0.455</v>
@@ -2737,7 +2740,7 @@
         <v>121.3</v>
       </c>
       <c r="G7" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H7">
         <v>0.596</v>
@@ -2772,7 +2775,7 @@
         <v>91.3</v>
       </c>
       <c r="G8" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H8">
         <v>0.5649999999999999</v>
@@ -2807,7 +2810,7 @@
         <v>63.6</v>
       </c>
       <c r="G9" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H9" t="s">
         <v>625</v>
@@ -2842,7 +2845,7 @@
         <v>81.59999999999999</v>
       </c>
       <c r="G10" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H10">
         <v>0.54</v>
@@ -2877,7 +2880,7 @@
         <v>72.7</v>
       </c>
       <c r="G11" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H11" t="s">
         <v>625</v>
@@ -2908,11 +2911,11 @@
       <c r="E12" t="s">
         <v>625</v>
       </c>
-      <c r="F12">
-        <v>56.2</v>
+      <c r="F12" t="s">
+        <v>706</v>
       </c>
       <c r="G12" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H12" t="s">
         <v>625</v>
@@ -2947,7 +2950,7 @@
         <v>117.6</v>
       </c>
       <c r="G13" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H13">
         <v>0.554</v>
@@ -2982,7 +2985,7 @@
         <v>78.59999999999999</v>
       </c>
       <c r="G14" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H14">
         <v>0.314</v>
@@ -3017,7 +3020,7 @@
         <v>82</v>
       </c>
       <c r="G15" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H15">
         <v>0.328</v>
@@ -3052,7 +3055,7 @@
         <v>46.1</v>
       </c>
       <c r="G16" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H16" t="s">
         <v>625</v>
@@ -3087,7 +3090,7 @@
         <v>71.5</v>
       </c>
       <c r="G17" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H17">
         <v>0.319</v>
@@ -3122,7 +3125,7 @@
         <v>64.90000000000001</v>
       </c>
       <c r="G18" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H18" t="s">
         <v>625</v>
@@ -3157,7 +3160,7 @@
         <v>77.3</v>
       </c>
       <c r="G19" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H19">
         <v>0.267</v>
@@ -3192,7 +3195,7 @@
         <v>56.3</v>
       </c>
       <c r="G20" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H20">
         <v>0.6929999999999999</v>
@@ -3227,7 +3230,7 @@
         <v>77</v>
       </c>
       <c r="G21" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H21">
         <v>0.196</v>
@@ -3262,7 +3265,7 @@
         <v>64.3</v>
       </c>
       <c r="G22" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H22">
         <v>0.304</v>
@@ -3297,7 +3300,7 @@
         <v>81</v>
       </c>
       <c r="G23" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H23">
         <v>0.326</v>
@@ -3332,7 +3335,7 @@
         <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H24" t="s">
         <v>625</v>
@@ -3367,7 +3370,7 @@
         <v>58.1</v>
       </c>
       <c r="G25" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H25">
         <v>0.257</v>
@@ -3398,11 +3401,11 @@
       <c r="E26" t="s">
         <v>625</v>
       </c>
-      <c r="F26">
-        <v>44.2</v>
+      <c r="F26" t="s">
+        <v>706</v>
       </c>
       <c r="G26" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H26" t="s">
         <v>625</v>
@@ -3437,7 +3440,7 @@
         <v>44.6</v>
       </c>
       <c r="G27" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H27">
         <v>0.516</v>
@@ -3472,7 +3475,7 @@
         <v>69.2</v>
       </c>
       <c r="G28" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H28" t="s">
         <v>625</v>
@@ -3507,7 +3510,7 @@
         <v>68.5</v>
       </c>
       <c r="G29" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H29">
         <v>0.38</v>
@@ -3542,7 +3545,7 @@
         <v>39.7</v>
       </c>
       <c r="G30" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H30" t="s">
         <v>625</v>
@@ -3577,7 +3580,7 @@
         <v>64.09999999999999</v>
       </c>
       <c r="G31" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H31" t="s">
         <v>625</v>
@@ -3612,7 +3615,7 @@
         <v>105.2</v>
       </c>
       <c r="G32" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H32">
         <v>0.544</v>
@@ -3647,7 +3650,7 @@
         <v>52.8</v>
       </c>
       <c r="G33" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H33" t="s">
         <v>625</v>
@@ -3682,7 +3685,7 @@
         <v>64.59999999999999</v>
       </c>
       <c r="G34" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H34" t="s">
         <v>625</v>
@@ -3717,7 +3720,7 @@
         <v>67.59999999999999</v>
       </c>
       <c r="G35" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H35" t="s">
         <v>625</v>
@@ -3748,8 +3751,8 @@
       <c r="E36" t="s">
         <v>675</v>
       </c>
-      <c r="F36">
-        <v>88.90000000000001</v>
+      <c r="F36" t="s">
+        <v>706</v>
       </c>
       <c r="G36" t="s">
         <v>706</v>
@@ -3787,7 +3790,7 @@
         <v>98.40000000000001</v>
       </c>
       <c r="G37" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H37">
         <v>0.516</v>
@@ -3822,7 +3825,7 @@
         <v>86.59999999999999</v>
       </c>
       <c r="G38" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H38">
         <v>0.35</v>
@@ -3857,7 +3860,7 @@
         <v>93.90000000000001</v>
       </c>
       <c r="G39" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H39" t="s">
         <v>625</v>
@@ -3892,7 +3895,7 @@
         <v>82.3</v>
       </c>
       <c r="G40" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H40">
         <v>0.261</v>
@@ -3927,7 +3930,7 @@
         <v>46.5</v>
       </c>
       <c r="G41" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H41" t="s">
         <v>625</v>
@@ -3962,7 +3965,7 @@
         <v>74</v>
       </c>
       <c r="G42" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H42">
         <v>0.287</v>
@@ -3997,7 +4000,7 @@
         <v>80.59999999999999</v>
       </c>
       <c r="G43" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H43">
         <v>0.15</v>
@@ -4032,7 +4035,7 @@
         <v>64.40000000000001</v>
       </c>
       <c r="G44" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H44" t="s">
         <v>625</v>
@@ -4067,7 +4070,7 @@
         <v>67</v>
       </c>
       <c r="G45" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H45" t="s">
         <v>625</v>
@@ -4102,7 +4105,7 @@
         <v>112.7</v>
       </c>
       <c r="G46" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H46">
         <v>0.354</v>
@@ -4137,7 +4140,7 @@
         <v>54.6</v>
       </c>
       <c r="G47" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H47" t="s">
         <v>625</v>
@@ -4172,7 +4175,7 @@
         <v>77.2</v>
       </c>
       <c r="G48" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H48">
         <v>0.308</v>
@@ -4207,7 +4210,7 @@
         <v>101.2</v>
       </c>
       <c r="G49" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H49">
         <v>0.339</v>
@@ -4242,7 +4245,7 @@
         <v>84.7</v>
       </c>
       <c r="G50" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H50">
         <v>0.431</v>
@@ -4277,7 +4280,7 @@
         <v>72.40000000000001</v>
       </c>
       <c r="G51" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H51">
         <v>0.456</v>
@@ -4312,7 +4315,7 @@
         <v>37.1</v>
       </c>
       <c r="G52" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H52" t="s">
         <v>625</v>
@@ -4347,7 +4350,7 @@
         <v>63.2</v>
       </c>
       <c r="G53" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H53" t="s">
         <v>625</v>
@@ -4382,7 +4385,7 @@
         <v>81.5</v>
       </c>
       <c r="G54" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H54">
         <v>0.339</v>
@@ -4413,8 +4416,8 @@
       <c r="E55" t="s">
         <v>64</v>
       </c>
-      <c r="F55">
-        <v>77.7</v>
+      <c r="F55" t="s">
+        <v>706</v>
       </c>
       <c r="G55" t="s">
         <v>706</v>
@@ -4452,7 +4455,7 @@
         <v>70.2</v>
       </c>
       <c r="G56" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H56">
         <v>0.231</v>
@@ -4487,7 +4490,7 @@
         <v>93.09999999999999</v>
       </c>
       <c r="G57" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H57">
         <v>0.308</v>
@@ -4518,8 +4521,8 @@
       <c r="E58" t="s">
         <v>625</v>
       </c>
-      <c r="F58">
-        <v>70</v>
+      <c r="F58" t="s">
+        <v>706</v>
       </c>
       <c r="G58" t="s">
         <v>706</v>
@@ -4557,7 +4560,7 @@
         <v>60.7</v>
       </c>
       <c r="G59" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H59" t="s">
         <v>625</v>
@@ -4592,7 +4595,7 @@
         <v>90.40000000000001</v>
       </c>
       <c r="G60" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H60">
         <v>0.569</v>
@@ -4627,7 +4630,7 @@
         <v>74.2</v>
       </c>
       <c r="G61" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H61">
         <v>0.365</v>
@@ -4662,7 +4665,7 @@
         <v>65.59999999999999</v>
       </c>
       <c r="G62" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H62" t="s">
         <v>625</v>
@@ -4697,7 +4700,7 @@
         <v>60.5</v>
       </c>
       <c r="G63" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H63" t="s">
         <v>625</v>
@@ -4732,7 +4735,7 @@
         <v>74.3</v>
       </c>
       <c r="G64" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H64">
         <v>0.285</v>
@@ -4767,7 +4770,7 @@
         <v>84.09999999999999</v>
       </c>
       <c r="G65" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H65">
         <v>0.337</v>
@@ -4802,7 +4805,7 @@
         <v>93.90000000000001</v>
       </c>
       <c r="G66" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H66">
         <v>0.335</v>
@@ -4837,7 +4840,7 @@
         <v>77.09999999999999</v>
       </c>
       <c r="G67" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H67">
         <v>0.381</v>
@@ -4872,7 +4875,7 @@
         <v>52.8</v>
       </c>
       <c r="G68" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H68" t="s">
         <v>625</v>
@@ -4907,7 +4910,7 @@
         <v>119.7</v>
       </c>
       <c r="G69" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H69">
         <v>0.475</v>
@@ -4942,7 +4945,7 @@
         <v>80.09999999999999</v>
       </c>
       <c r="G70" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H70">
         <v>0.626</v>
@@ -4977,7 +4980,7 @@
         <v>41.7</v>
       </c>
       <c r="G71" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H71" t="s">
         <v>625</v>
@@ -5008,11 +5011,11 @@
       <c r="E72" t="s">
         <v>625</v>
       </c>
-      <c r="F72">
-        <v>43.9</v>
+      <c r="F72" t="s">
+        <v>706</v>
       </c>
       <c r="G72" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H72" t="s">
         <v>625</v>
@@ -5047,7 +5050,7 @@
         <v>44.8</v>
       </c>
       <c r="G73" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H73" t="s">
         <v>625</v>
@@ -5082,7 +5085,7 @@
         <v>82.7</v>
       </c>
       <c r="G74" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H74">
         <v>0.434</v>
@@ -5117,7 +5120,7 @@
         <v>78.8</v>
       </c>
       <c r="G75" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H75">
         <v>0.293</v>
@@ -5152,7 +5155,7 @@
         <v>63.7</v>
       </c>
       <c r="G76" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H76" t="s">
         <v>625</v>
@@ -5183,8 +5186,8 @@
       <c r="E77" t="s">
         <v>163</v>
       </c>
-      <c r="F77">
-        <v>95.59999999999999</v>
+      <c r="F77" t="s">
+        <v>706</v>
       </c>
       <c r="G77" t="s">
         <v>706</v>
@@ -5222,7 +5225,7 @@
         <v>54</v>
       </c>
       <c r="G78" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H78" t="s">
         <v>625</v>
@@ -5257,7 +5260,7 @@
         <v>51.1</v>
       </c>
       <c r="G79" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H79" t="s">
         <v>625</v>
@@ -5292,7 +5295,7 @@
         <v>44.8</v>
       </c>
       <c r="G80" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H80" t="s">
         <v>625</v>
@@ -5327,7 +5330,7 @@
         <v>44.9</v>
       </c>
       <c r="G81" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H81" t="s">
         <v>625</v>
@@ -5362,7 +5365,7 @@
         <v>61</v>
       </c>
       <c r="G82" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H82">
         <v>0.179</v>
@@ -5393,8 +5396,8 @@
       <c r="E83" t="s">
         <v>625</v>
       </c>
-      <c r="F83">
-        <v>79.40000000000001</v>
+      <c r="F83" t="s">
+        <v>706</v>
       </c>
       <c r="G83" t="s">
         <v>706</v>
@@ -5432,7 +5435,7 @@
         <v>84.40000000000001</v>
       </c>
       <c r="G84" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H84">
         <v>0.425</v>
@@ -5467,7 +5470,7 @@
         <v>88.09999999999999</v>
       </c>
       <c r="G85" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H85">
         <v>0.439</v>
@@ -5502,7 +5505,7 @@
         <v>86.90000000000001</v>
       </c>
       <c r="G86" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H86">
         <v>0.535</v>
@@ -5537,7 +5540,7 @@
         <v>99.8</v>
       </c>
       <c r="G87" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H87">
         <v>0.192</v>
@@ -5572,7 +5575,7 @@
         <v>92.90000000000001</v>
       </c>
       <c r="G88" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H88">
         <v>0.394</v>
@@ -5607,7 +5610,7 @@
         <v>107.2</v>
       </c>
       <c r="G89" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H89">
         <v>0.46</v>
@@ -5642,7 +5645,7 @@
         <v>46.7</v>
       </c>
       <c r="G90" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H90" t="s">
         <v>625</v>
@@ -5677,7 +5680,7 @@
         <v>88.59999999999999</v>
       </c>
       <c r="G91" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H91">
         <v>0.067</v>
@@ -5712,7 +5715,7 @@
         <v>68.8</v>
       </c>
       <c r="G92" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H92" t="s">
         <v>625</v>
@@ -5747,7 +5750,7 @@
         <v>70.59999999999999</v>
       </c>
       <c r="G93" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H93">
         <v>0.333</v>
@@ -5782,7 +5785,7 @@
         <v>69.8</v>
       </c>
       <c r="G94" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H94" t="s">
         <v>625</v>
@@ -5817,7 +5820,7 @@
         <v>80.2</v>
       </c>
       <c r="G95" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H95">
         <v>0.265</v>
@@ -5852,7 +5855,7 @@
         <v>68.7</v>
       </c>
       <c r="G96" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H96" t="s">
         <v>625</v>
@@ -5887,7 +5890,7 @@
         <v>112.4</v>
       </c>
       <c r="G97" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H97">
         <v>0.573</v>
@@ -5922,7 +5925,7 @@
         <v>49.1</v>
       </c>
       <c r="G98" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H98" t="s">
         <v>625</v>
@@ -5957,7 +5960,7 @@
         <v>62.5</v>
       </c>
       <c r="G99" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H99" t="s">
         <v>625</v>
@@ -5992,7 +5995,7 @@
         <v>70.2</v>
       </c>
       <c r="G100" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H100" t="s">
         <v>625</v>
@@ -6027,7 +6030,7 @@
         <v>96.09999999999999</v>
       </c>
       <c r="G101" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H101">
         <v>0.553</v>
@@ -6062,7 +6065,7 @@
         <v>40.7</v>
       </c>
       <c r="G102" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H102" t="s">
         <v>625</v>
@@ -6097,7 +6100,7 @@
         <v>82.2</v>
       </c>
       <c r="G103" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H103">
         <v>0.478</v>
@@ -6132,7 +6135,7 @@
         <v>75</v>
       </c>
       <c r="G104" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H104">
         <v>0.44</v>
@@ -6167,7 +6170,7 @@
         <v>71.59999999999999</v>
       </c>
       <c r="G105" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H105" t="s">
         <v>625</v>
@@ -6202,7 +6205,7 @@
         <v>34.3</v>
       </c>
       <c r="G106" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H106" t="s">
         <v>625</v>
@@ -6233,11 +6236,11 @@
       <c r="E107" t="s">
         <v>625</v>
       </c>
-      <c r="F107">
-        <v>28</v>
+      <c r="F107" t="s">
+        <v>706</v>
       </c>
       <c r="G107" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H107" t="s">
         <v>625</v>
@@ -6272,7 +6275,7 @@
         <v>68.90000000000001</v>
       </c>
       <c r="G108" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H108">
         <v>0.351</v>
@@ -6307,7 +6310,7 @@
         <v>94.59999999999999</v>
       </c>
       <c r="G109" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H109">
         <v>0.345</v>
@@ -6342,7 +6345,7 @@
         <v>32.5</v>
       </c>
       <c r="G110" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H110">
         <v>0.34</v>
@@ -6377,7 +6380,7 @@
         <v>93</v>
       </c>
       <c r="G111" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H111">
         <v>0.245</v>
@@ -6412,7 +6415,7 @@
         <v>52.5</v>
       </c>
       <c r="G112" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H112" t="s">
         <v>625</v>
@@ -6447,7 +6450,7 @@
         <v>94.7</v>
       </c>
       <c r="G113" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H113">
         <v>0.394</v>
@@ -6482,7 +6485,7 @@
         <v>80.5</v>
       </c>
       <c r="G114" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H114">
         <v>0.366</v>
@@ -6517,7 +6520,7 @@
         <v>56.7</v>
       </c>
       <c r="G115" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H115" t="s">
         <v>625</v>
@@ -6552,7 +6555,7 @@
         <v>66.7</v>
       </c>
       <c r="G116" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H116" t="s">
         <v>625</v>
@@ -6587,7 +6590,7 @@
         <v>69.09999999999999</v>
       </c>
       <c r="G117" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H117" t="s">
         <v>625</v>
@@ -6622,7 +6625,7 @@
         <v>47.5</v>
       </c>
       <c r="G118" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H118" t="s">
         <v>625</v>
@@ -6657,7 +6660,7 @@
         <v>83.59999999999999</v>
       </c>
       <c r="G119" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H119">
         <v>0.35</v>
@@ -6692,7 +6695,7 @@
         <v>103.6</v>
       </c>
       <c r="G120" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H120">
         <v>0.431</v>
@@ -6727,7 +6730,7 @@
         <v>51.2</v>
       </c>
       <c r="G121" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H121" t="s">
         <v>625</v>
@@ -6762,7 +6765,7 @@
         <v>35.6</v>
       </c>
       <c r="G122" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H122" t="s">
         <v>625</v>
@@ -6797,7 +6800,7 @@
         <v>101.8</v>
       </c>
       <c r="G123" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H123">
         <v>0.327</v>
@@ -6832,7 +6835,7 @@
         <v>93.3</v>
       </c>
       <c r="G124" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H124">
         <v>0.352</v>
@@ -6867,7 +6870,7 @@
         <v>64.40000000000001</v>
       </c>
       <c r="G125" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H125">
         <v>0.315</v>
@@ -6902,7 +6905,7 @@
         <v>93.59999999999999</v>
       </c>
       <c r="G126" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H126">
         <v>0.44</v>
@@ -6937,7 +6940,7 @@
         <v>109</v>
       </c>
       <c r="G127" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H127">
         <v>0.357</v>
@@ -6972,7 +6975,7 @@
         <v>64.8</v>
       </c>
       <c r="G128" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H128" t="s">
         <v>625</v>
@@ -7007,7 +7010,7 @@
         <v>93.5</v>
       </c>
       <c r="G129" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H129">
         <v>0.508</v>
@@ -7042,7 +7045,7 @@
         <v>67.40000000000001</v>
       </c>
       <c r="G130" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H130" t="s">
         <v>625</v>
@@ -7077,7 +7080,7 @@
         <v>44.6</v>
       </c>
       <c r="G131" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H131" t="s">
         <v>625</v>
@@ -7112,7 +7115,7 @@
         <v>-18.2</v>
       </c>
       <c r="G132" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="H132" t="s">
         <v>625</v>
@@ -7147,7 +7150,7 @@
         <v>72.5</v>
       </c>
       <c r="G133" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H133" t="s">
         <v>625</v>
@@ -7182,7 +7185,7 @@
         <v>94.3</v>
       </c>
       <c r="G134" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H134">
         <v>0.386</v>
@@ -7217,7 +7220,7 @@
         <v>70.3</v>
       </c>
       <c r="G135" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H135" t="s">
         <v>625</v>
@@ -7252,7 +7255,7 @@
         <v>81.59999999999999</v>
       </c>
       <c r="G136" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H136">
         <v>0.751</v>
@@ -7287,7 +7290,7 @@
         <v>89.3</v>
       </c>
       <c r="G137" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H137">
         <v>0.338</v>
@@ -7322,7 +7325,7 @@
         <v>89.90000000000001</v>
       </c>
       <c r="G138" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H138">
         <v>0.302</v>
@@ -7357,7 +7360,7 @@
         <v>111.3</v>
       </c>
       <c r="G139" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H139">
         <v>0.72</v>
@@ -7392,7 +7395,7 @@
         <v>46.2</v>
       </c>
       <c r="G140" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H140" t="s">
         <v>625</v>
@@ -7427,7 +7430,7 @@
         <v>63.9</v>
       </c>
       <c r="G141" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H141">
         <v>0.206</v>
@@ -7462,7 +7465,7 @@
         <v>50.7</v>
       </c>
       <c r="G142" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H142" t="s">
         <v>625</v>
@@ -7497,7 +7500,7 @@
         <v>38.9</v>
       </c>
       <c r="G143" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H143" t="s">
         <v>625</v>
@@ -7532,7 +7535,7 @@
         <v>88.09999999999999</v>
       </c>
       <c r="G144" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H144">
         <v>0.374</v>
@@ -7567,7 +7570,7 @@
         <v>72</v>
       </c>
       <c r="G145" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H145" t="s">
         <v>625</v>
@@ -7602,7 +7605,7 @@
         <v>93.90000000000001</v>
       </c>
       <c r="G146" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H146">
         <v>0.285</v>
@@ -7637,7 +7640,7 @@
         <v>45.2</v>
       </c>
       <c r="G147" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H147" t="s">
         <v>625</v>
@@ -7672,7 +7675,7 @@
         <v>75.40000000000001</v>
       </c>
       <c r="G148" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H148">
         <v>0.25</v>
@@ -7707,7 +7710,7 @@
         <v>66.3</v>
       </c>
       <c r="G149" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H149" t="s">
         <v>625</v>
@@ -7742,7 +7745,7 @@
         <v>52.4</v>
       </c>
       <c r="G150" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H150" t="s">
         <v>625</v>
@@ -7777,7 +7780,7 @@
         <v>59.4</v>
       </c>
       <c r="G151" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H151" t="s">
         <v>625</v>
@@ -7812,7 +7815,7 @@
         <v>65.5</v>
       </c>
       <c r="G152" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H152" t="s">
         <v>625</v>
@@ -7847,7 +7850,7 @@
         <v>95.2</v>
       </c>
       <c r="G153" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H153">
         <v>0.481</v>
@@ -7882,7 +7885,7 @@
         <v>79</v>
       </c>
       <c r="G154" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H154">
         <v>0.586</v>
@@ -7917,7 +7920,7 @@
         <v>74.90000000000001</v>
       </c>
       <c r="G155" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H155">
         <v>0.41</v>
@@ -7952,7 +7955,7 @@
         <v>53.4</v>
       </c>
       <c r="G156" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H156" t="s">
         <v>625</v>
@@ -7987,7 +7990,7 @@
         <v>92.5</v>
       </c>
       <c r="G157" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H157">
         <v>0.312</v>
@@ -8022,7 +8025,7 @@
         <v>56.2</v>
       </c>
       <c r="G158" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H158" t="s">
         <v>625</v>
@@ -8057,7 +8060,7 @@
         <v>88.59999999999999</v>
       </c>
       <c r="G159" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H159">
         <v>0.427</v>
@@ -8088,11 +8091,11 @@
       <c r="E160" t="s">
         <v>238</v>
       </c>
-      <c r="F160">
-        <v>59.7</v>
+      <c r="F160" t="s">
+        <v>706</v>
       </c>
       <c r="G160" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H160">
         <v>0.372</v>
@@ -8127,7 +8130,7 @@
         <v>83.3</v>
       </c>
       <c r="G161" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H161">
         <v>0.411</v>
@@ -8162,7 +8165,7 @@
         <v>62.1</v>
       </c>
       <c r="G162" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H162">
         <v>0.318</v>
@@ -8197,7 +8200,7 @@
         <v>99.5</v>
       </c>
       <c r="G163" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H163" t="s">
         <v>625</v>
@@ -8232,7 +8235,7 @@
         <v>41.9</v>
       </c>
       <c r="G164" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H164" t="s">
         <v>625</v>
@@ -8267,7 +8270,7 @@
         <v>64.5</v>
       </c>
       <c r="G165" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H165" t="s">
         <v>625</v>
@@ -8302,7 +8305,7 @@
         <v>46.2</v>
       </c>
       <c r="G166" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H166">
         <v>0.353</v>
@@ -8337,7 +8340,7 @@
         <v>80.3</v>
       </c>
       <c r="G167" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H167" t="s">
         <v>625</v>
@@ -8372,7 +8375,7 @@
         <v>67.59999999999999</v>
       </c>
       <c r="G168" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H168" t="s">
         <v>625</v>
@@ -8407,7 +8410,7 @@
         <v>93.09999999999999</v>
       </c>
       <c r="G169" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H169">
         <v>0.409</v>
@@ -8442,7 +8445,7 @@
         <v>26.2</v>
       </c>
       <c r="G170" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H170" t="s">
         <v>625</v>
@@ -8477,7 +8480,7 @@
         <v>68.5</v>
       </c>
       <c r="G171" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H171">
         <v>0.444</v>
@@ -8512,7 +8515,7 @@
         <v>51.8</v>
       </c>
       <c r="G172" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H172" t="s">
         <v>625</v>
@@ -8547,7 +8550,7 @@
         <v>83</v>
       </c>
       <c r="G173" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H173">
         <v>0.275</v>
@@ -8582,7 +8585,7 @@
         <v>100.6</v>
       </c>
       <c r="G174" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H174">
         <v>0.702</v>
@@ -8617,7 +8620,7 @@
         <v>57.7</v>
       </c>
       <c r="G175" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H175">
         <v>0.491</v>
@@ -8652,7 +8655,7 @@
         <v>25.5</v>
       </c>
       <c r="G176" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="H176">
         <v>0.325</v>
@@ -8687,7 +8690,7 @@
         <v>77.90000000000001</v>
       </c>
       <c r="G177" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H177">
         <v>0.437</v>
@@ -8722,7 +8725,7 @@
         <v>72.40000000000001</v>
       </c>
       <c r="G178" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H178">
         <v>0.225</v>
@@ -8757,7 +8760,7 @@
         <v>52.6</v>
       </c>
       <c r="G179" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H179" t="s">
         <v>625</v>
@@ -8792,7 +8795,7 @@
         <v>70.59999999999999</v>
       </c>
       <c r="G180" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H180" t="s">
         <v>625</v>
@@ -8827,7 +8830,7 @@
         <v>89.5</v>
       </c>
       <c r="G181" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H181">
         <v>0.483</v>
@@ -8858,8 +8861,8 @@
       <c r="E182" t="s">
         <v>191</v>
       </c>
-      <c r="F182">
-        <v>69.5</v>
+      <c r="F182" t="s">
+        <v>706</v>
       </c>
       <c r="G182" t="s">
         <v>706</v>
@@ -8932,7 +8935,7 @@
         <v>88.2</v>
       </c>
       <c r="G184" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H184">
         <v>0.414</v>
@@ -8967,7 +8970,7 @@
         <v>99.5</v>
       </c>
       <c r="G185" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H185">
         <v>0.495</v>
@@ -9002,7 +9005,7 @@
         <v>93.90000000000001</v>
       </c>
       <c r="G186" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H186" t="s">
         <v>625</v>
@@ -9037,7 +9040,7 @@
         <v>90.2</v>
       </c>
       <c r="G187" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H187">
         <v>0.407</v>
@@ -9072,7 +9075,7 @@
         <v>87.59999999999999</v>
       </c>
       <c r="G188" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H188">
         <v>0.49</v>
@@ -9107,7 +9110,7 @@
         <v>68.59999999999999</v>
       </c>
       <c r="G189" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H189">
         <v>0.166</v>
@@ -9142,7 +9145,7 @@
         <v>-6.2</v>
       </c>
       <c r="G190" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="H190" t="s">
         <v>625</v>
@@ -9177,7 +9180,7 @@
         <v>55.1</v>
       </c>
       <c r="G191" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H191" t="s">
         <v>625</v>
@@ -9212,7 +9215,7 @@
         <v>49.9</v>
       </c>
       <c r="G192" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H192" t="s">
         <v>625</v>
@@ -9247,7 +9250,7 @@
         <v>98.3</v>
       </c>
       <c r="G193" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H193" t="s">
         <v>625</v>
@@ -9282,7 +9285,7 @@
         <v>38.4</v>
       </c>
       <c r="G194" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H194" t="s">
         <v>625</v>
@@ -9317,7 +9320,7 @@
         <v>114</v>
       </c>
       <c r="G195" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H195">
         <v>0.719</v>
@@ -9352,7 +9355,7 @@
         <v>68.59999999999999</v>
       </c>
       <c r="G196" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H196">
         <v>0.358</v>
@@ -9387,7 +9390,7 @@
         <v>51</v>
       </c>
       <c r="G197" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H197" t="s">
         <v>625</v>
@@ -9422,7 +9425,7 @@
         <v>85</v>
       </c>
       <c r="G198" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H198" t="s">
         <v>625</v>
@@ -9457,7 +9460,7 @@
         <v>109</v>
       </c>
       <c r="G199" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H199">
         <v>0.492</v>
@@ -9488,8 +9491,8 @@
       <c r="E200" t="s">
         <v>209</v>
       </c>
-      <c r="F200">
-        <v>76</v>
+      <c r="F200" t="s">
+        <v>706</v>
       </c>
       <c r="G200" t="s">
         <v>706</v>
@@ -9527,7 +9530,7 @@
         <v>14.8</v>
       </c>
       <c r="G201" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="H201" t="s">
         <v>625</v>
@@ -9562,7 +9565,7 @@
         <v>64</v>
       </c>
       <c r="G202" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H202" t="s">
         <v>625</v>
@@ -9597,7 +9600,7 @@
         <v>59</v>
       </c>
       <c r="G203" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H203">
         <v>0.255</v>
@@ -9632,7 +9635,7 @@
         <v>77.59999999999999</v>
       </c>
       <c r="G204" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H204" t="s">
         <v>625</v>
@@ -9667,7 +9670,7 @@
         <v>79.40000000000001</v>
       </c>
       <c r="G205" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H205" t="s">
         <v>625</v>
@@ -9702,7 +9705,7 @@
         <v>111.7</v>
       </c>
       <c r="G206" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H206">
         <v>0.34</v>
@@ -9737,7 +9740,7 @@
         <v>83.7</v>
       </c>
       <c r="G207" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H207">
         <v>0.353</v>
@@ -9772,7 +9775,7 @@
         <v>82.5</v>
       </c>
       <c r="G208" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H208">
         <v>0.314</v>
@@ -9807,7 +9810,7 @@
         <v>77.09999999999999</v>
       </c>
       <c r="G209" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H209">
         <v>0.172</v>
@@ -9842,7 +9845,7 @@
         <v>72.40000000000001</v>
       </c>
       <c r="G210" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H210">
         <v>0.4</v>
@@ -9877,7 +9880,7 @@
         <v>76.40000000000001</v>
       </c>
       <c r="G211" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H211">
         <v>0.255</v>
@@ -9912,7 +9915,7 @@
         <v>96.59999999999999</v>
       </c>
       <c r="G212" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H212">
         <v>0.235</v>
@@ -9947,7 +9950,7 @@
         <v>95.09999999999999</v>
       </c>
       <c r="G213" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H213">
         <v>0.53</v>
@@ -9982,7 +9985,7 @@
         <v>64.3</v>
       </c>
       <c r="G214" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H214">
         <v>0.236</v>
@@ -10017,7 +10020,7 @@
         <v>50.1</v>
       </c>
       <c r="G215" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H215" t="s">
         <v>625</v>
@@ -10052,7 +10055,7 @@
         <v>97.90000000000001</v>
       </c>
       <c r="G216" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H216">
         <v>0.397</v>
@@ -10087,7 +10090,7 @@
         <v>106.7</v>
       </c>
       <c r="G217" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H217">
         <v>0.4</v>
@@ -10122,7 +10125,7 @@
         <v>57.2</v>
       </c>
       <c r="G218" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H218" t="s">
         <v>625</v>
@@ -10157,7 +10160,7 @@
         <v>83.59999999999999</v>
       </c>
       <c r="G219" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H219">
         <v>0.373</v>
@@ -10192,7 +10195,7 @@
         <v>94.7</v>
       </c>
       <c r="G220" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H220">
         <v>0.485</v>
@@ -10227,7 +10230,7 @@
         <v>96.3</v>
       </c>
       <c r="G221" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H221">
         <v>0.481</v>
@@ -10262,7 +10265,7 @@
         <v>54.6</v>
       </c>
       <c r="G222" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H222" t="s">
         <v>625</v>
@@ -10297,7 +10300,7 @@
         <v>67.59999999999999</v>
       </c>
       <c r="G223" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H223">
         <v>0.188</v>
@@ -10332,7 +10335,7 @@
         <v>30.2</v>
       </c>
       <c r="G224" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H224" t="s">
         <v>625</v>
@@ -10367,7 +10370,7 @@
         <v>83.8</v>
       </c>
       <c r="G225" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H225">
         <v>0.335</v>
@@ -10402,7 +10405,7 @@
         <v>70.40000000000001</v>
       </c>
       <c r="G226" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H226">
         <v>0.211</v>
@@ -10437,7 +10440,7 @@
         <v>67.8</v>
       </c>
       <c r="G227" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="H227">
         <v>0.404</v>
@@ -10472,7 +10475,7 @@
         <v>85.8</v>
       </c>
       <c r="G228" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H228">
         <v>0.458</v>
@@ -10507,7 +10510,7 @@
         <v>93.59999999999999</v>
       </c>
       <c r="G229" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="H229">
         <v>0.502</v>

</xml_diff>